<commit_message>
Update in test case file
</commit_message>
<xml_diff>
--- a/Test_Cases_TourToPK.xlsx
+++ b/Test_Cases_TourToPK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\University_Study\Final Year Project\FYP-2\Project\TourToPK-Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2DC76D-0549-43E6-86AD-6EC5B78C5E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B22378-3A1E-4FC4-B645-424D0584E19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{EDDAB5D1-2AE6-43D3-8E96-778F7AC8E49F}"/>
+    <workbookView xWindow="7920" yWindow="0" windowWidth="12570" windowHeight="10920" xr2:uid="{EDDAB5D1-2AE6-43D3-8E96-778F7AC8E49F}"/>
   </bookViews>
   <sheets>
     <sheet name="test_cases" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="303">
   <si>
     <t>Test_Case_ID</t>
   </si>
@@ -107,13 +107,866 @@
   </si>
   <si>
     <t>Button Disable</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>logic with the valid data set</t>
+  </si>
+  <si>
+    <t>The system should log in to  the app and navigate to the home screen</t>
+  </si>
+  <si>
+    <t>as expected</t>
+  </si>
+  <si>
+    <t>tc_toutpk_01</t>
+  </si>
+  <si>
+    <t>tc_toutpk_02</t>
+  </si>
+  <si>
+    <t>tc_toutpk_03</t>
+  </si>
+  <si>
+    <t>tc_toutpk_04</t>
+  </si>
+  <si>
+    <t>tc_toutpk_05</t>
+  </si>
+  <si>
+    <t>tc_toutpk_06</t>
+  </si>
+  <si>
+    <t>tc_toutpk_07</t>
+  </si>
+  <si>
+    <t>tc_toutpk_08</t>
+  </si>
+  <si>
+    <t>tc_toutpk_09</t>
+  </si>
+  <si>
+    <t>tc_toutpk_10</t>
+  </si>
+  <si>
+    <t>tc_toutpk_11</t>
+  </si>
+  <si>
+    <t>tc_toutpk_12</t>
+  </si>
+  <si>
+    <t>tc_toutpk_13</t>
+  </si>
+  <si>
+    <t>tc_toutpk_14</t>
+  </si>
+  <si>
+    <t>tc_toutpk_15</t>
+  </si>
+  <si>
+    <t>tc_toutpk_16</t>
+  </si>
+  <si>
+    <t>tc_toutpk_17</t>
+  </si>
+  <si>
+    <t>tc_toutpk_18</t>
+  </si>
+  <si>
+    <t>tc_toutpk_19</t>
+  </si>
+  <si>
+    <t>tc_toutpk_20</t>
+  </si>
+  <si>
+    <t>tc_toutpk_21</t>
+  </si>
+  <si>
+    <t>tc_toutpk_22</t>
+  </si>
+  <si>
+    <t>tc_toutpk_23</t>
+  </si>
+  <si>
+    <t>tc_toutpk_24</t>
+  </si>
+  <si>
+    <t>tc_toutpk_25</t>
+  </si>
+  <si>
+    <t>tc_toutpk_26</t>
+  </si>
+  <si>
+    <t>tc_toutpk_27</t>
+  </si>
+  <si>
+    <t>tc_toutpk_28</t>
+  </si>
+  <si>
+    <t>tc_toutpk_29</t>
+  </si>
+  <si>
+    <t>tc_toutpk_30</t>
+  </si>
+  <si>
+    <t>tc_toutpk_31</t>
+  </si>
+  <si>
+    <t>tc_toutpk_32</t>
+  </si>
+  <si>
+    <t>tc_toutpk_33</t>
+  </si>
+  <si>
+    <t>tc_toutpk_34</t>
+  </si>
+  <si>
+    <t>tc_toutpk_35</t>
+  </si>
+  <si>
+    <t>tc_toutpk_36</t>
+  </si>
+  <si>
+    <t>tc_toutpk_37</t>
+  </si>
+  <si>
+    <t>tc_toutpk_38</t>
+  </si>
+  <si>
+    <t>tc_toutpk_39</t>
+  </si>
+  <si>
+    <t>tc_toutpk_40</t>
+  </si>
+  <si>
+    <t>tc_toutpk_41</t>
+  </si>
+  <si>
+    <t>tc_toutpk_42</t>
+  </si>
+  <si>
+    <t>tc_toutpk_43</t>
+  </si>
+  <si>
+    <t>tc_toutpk_44</t>
+  </si>
+  <si>
+    <t>tc_toutpk_45</t>
+  </si>
+  <si>
+    <t>tc_toutpk_46</t>
+  </si>
+  <si>
+    <t>tc_toutpk_47</t>
+  </si>
+  <si>
+    <t>tc_toutpk_48</t>
+  </si>
+  <si>
+    <t>tc_toutpk_49</t>
+  </si>
+  <si>
+    <t>tc_toutpk_50</t>
+  </si>
+  <si>
+    <t>tc_toutpk_51</t>
+  </si>
+  <si>
+    <t>tc_toutpk_52</t>
+  </si>
+  <si>
+    <t>tc_toutpk_53</t>
+  </si>
+  <si>
+    <t>tc_toutpk_54</t>
+  </si>
+  <si>
+    <t>tc_toutpk_55</t>
+  </si>
+  <si>
+    <t>tc_toutpk_56</t>
+  </si>
+  <si>
+    <t>tc_toutpk_57</t>
+  </si>
+  <si>
+    <t>tc_toutpk_58</t>
+  </si>
+  <si>
+    <t>tc_toutpk_59</t>
+  </si>
+  <si>
+    <t>tc_toutpk_60</t>
+  </si>
+  <si>
+    <t>tc_toutpk_61</t>
+  </si>
+  <si>
+    <t>tc_toutpk_62</t>
+  </si>
+  <si>
+    <t>tc_toutpk_63</t>
+  </si>
+  <si>
+    <t>tc_toutpk_64</t>
+  </si>
+  <si>
+    <t>tc_toutpk_65</t>
+  </si>
+  <si>
+    <t>tc_toutpk_66</t>
+  </si>
+  <si>
+    <t>tc_toutpk_67</t>
+  </si>
+  <si>
+    <t>tc_toutpk_68</t>
+  </si>
+  <si>
+    <t>tc_toutpk_69</t>
+  </si>
+  <si>
+    <t>tc_toutpk_70</t>
+  </si>
+  <si>
+    <t>tc_toutpk_71</t>
+  </si>
+  <si>
+    <t>tc_toutpk_72</t>
+  </si>
+  <si>
+    <t>tc_toutpk_73</t>
+  </si>
+  <si>
+    <t>tc_toutpk_74</t>
+  </si>
+  <si>
+    <t>tc_toutpk_75</t>
+  </si>
+  <si>
+    <t>tc_toutpk_76</t>
+  </si>
+  <si>
+    <t>tc_toutpk_77</t>
+  </si>
+  <si>
+    <t>tc_toutpk_78</t>
+  </si>
+  <si>
+    <t>tc_toutpk_79</t>
+  </si>
+  <si>
+    <t>tc_toutpk_80</t>
+  </si>
+  <si>
+    <t>tc_toutpk_81</t>
+  </si>
+  <si>
+    <t>tc_toutpk_82</t>
+  </si>
+  <si>
+    <t>tc_toutpk_83</t>
+  </si>
+  <si>
+    <t>tc_toutpk_84</t>
+  </si>
+  <si>
+    <t>tc_toutpk_85</t>
+  </si>
+  <si>
+    <t>tc_toutpk_86</t>
+  </si>
+  <si>
+    <t>tc_toutpk_87</t>
+  </si>
+  <si>
+    <t>tc_toutpk_88</t>
+  </si>
+  <si>
+    <t>tc_toutpk_89</t>
+  </si>
+  <si>
+    <t>tc_toutpk_90</t>
+  </si>
+  <si>
+    <t>tc_toutpk_91</t>
+  </si>
+  <si>
+    <t>tc_toutpk_92</t>
+  </si>
+  <si>
+    <t>tc_toutpk_93</t>
+  </si>
+  <si>
+    <t>tc_toutpk_94</t>
+  </si>
+  <si>
+    <t>tc_toutpk_95</t>
+  </si>
+  <si>
+    <t>tc_toutpk_96</t>
+  </si>
+  <si>
+    <t>tc_toutpk_97</t>
+  </si>
+  <si>
+    <t>tc_toutpk_98</t>
+  </si>
+  <si>
+    <t>tc_toutpk_99</t>
+  </si>
+  <si>
+    <t>tc_toutpk_100</t>
+  </si>
+  <si>
+    <t>tc_toutpk_101</t>
+  </si>
+  <si>
+    <t>tc_toutpk_102</t>
+  </si>
+  <si>
+    <t>tc_toutpk_103</t>
+  </si>
+  <si>
+    <t>tc_toutpk_104</t>
+  </si>
+  <si>
+    <t>tc_toutpk_105</t>
+  </si>
+  <si>
+    <t>tc_toutpk_106</t>
+  </si>
+  <si>
+    <t>tc_toutpk_107</t>
+  </si>
+  <si>
+    <t>tc_toutpk_108</t>
+  </si>
+  <si>
+    <t>tc_toutpk_109</t>
+  </si>
+  <si>
+    <t>tc_toutpk_110</t>
+  </si>
+  <si>
+    <t>tc_toutpk_111</t>
+  </si>
+  <si>
+    <t>tc_toutpk_112</t>
+  </si>
+  <si>
+    <t>tc_toutpk_113</t>
+  </si>
+  <si>
+    <t>tc_toutpk_114</t>
+  </si>
+  <si>
+    <t>tc_toutpk_115</t>
+  </si>
+  <si>
+    <t>tc_toutpk_116</t>
+  </si>
+  <si>
+    <t>tc_toutpk_117</t>
+  </si>
+  <si>
+    <t>tc_toutpk_118</t>
+  </si>
+  <si>
+    <t>tc_toutpk_119</t>
+  </si>
+  <si>
+    <t>tc_toutpk_120</t>
+  </si>
+  <si>
+    <t>tc_toutpk_121</t>
+  </si>
+  <si>
+    <t>tc_toutpk_122</t>
+  </si>
+  <si>
+    <t>tc_toutpk_123</t>
+  </si>
+  <si>
+    <t>tc_toutpk_124</t>
+  </si>
+  <si>
+    <t>tc_toutpk_125</t>
+  </si>
+  <si>
+    <t>tc_toutpk_126</t>
+  </si>
+  <si>
+    <t>tc_toutpk_127</t>
+  </si>
+  <si>
+    <t>tc_toutpk_128</t>
+  </si>
+  <si>
+    <t>tc_toutpk_129</t>
+  </si>
+  <si>
+    <t>tc_toutpk_130</t>
+  </si>
+  <si>
+    <t>tc_toutpk_131</t>
+  </si>
+  <si>
+    <t>tc_toutpk_132</t>
+  </si>
+  <si>
+    <t>tc_toutpk_133</t>
+  </si>
+  <si>
+    <t>tc_toutpk_134</t>
+  </si>
+  <si>
+    <t>tc_toutpk_135</t>
+  </si>
+  <si>
+    <t>tc_toutpk_136</t>
+  </si>
+  <si>
+    <t>tc_toutpk_137</t>
+  </si>
+  <si>
+    <t>tc_toutpk_138</t>
+  </si>
+  <si>
+    <t>tc_toutpk_139</t>
+  </si>
+  <si>
+    <t>tc_toutpk_140</t>
+  </si>
+  <si>
+    <t>tc_toutpk_141</t>
+  </si>
+  <si>
+    <t>tc_toutpk_142</t>
+  </si>
+  <si>
+    <t>tc_toutpk_143</t>
+  </si>
+  <si>
+    <t>tc_toutpk_144</t>
+  </si>
+  <si>
+    <t>tc_toutpk_145</t>
+  </si>
+  <si>
+    <t>tc_toutpk_146</t>
+  </si>
+  <si>
+    <t>tc_toutpk_147</t>
+  </si>
+  <si>
+    <t>tc_toutpk_148</t>
+  </si>
+  <si>
+    <t>tc_toutpk_149</t>
+  </si>
+  <si>
+    <t>tc_toutpk_150</t>
+  </si>
+  <si>
+    <t>tc_toutpk_151</t>
+  </si>
+  <si>
+    <t>tc_toutpk_152</t>
+  </si>
+  <si>
+    <t>tc_toutpk_153</t>
+  </si>
+  <si>
+    <t>tc_toutpk_154</t>
+  </si>
+  <si>
+    <t>tc_toutpk_155</t>
+  </si>
+  <si>
+    <t>tc_toutpk_156</t>
+  </si>
+  <si>
+    <t>tc_toutpk_157</t>
+  </si>
+  <si>
+    <t>tc_toutpk_158</t>
+  </si>
+  <si>
+    <t>tc_toutpk_159</t>
+  </si>
+  <si>
+    <t>tc_toutpk_160</t>
+  </si>
+  <si>
+    <t>tc_toutpk_161</t>
+  </si>
+  <si>
+    <t>tc_toutpk_162</t>
+  </si>
+  <si>
+    <t>tc_toutpk_163</t>
+  </si>
+  <si>
+    <t>tc_toutpk_164</t>
+  </si>
+  <si>
+    <t>tc_toutpk_165</t>
+  </si>
+  <si>
+    <t>tc_toutpk_166</t>
+  </si>
+  <si>
+    <t>tc_toutpk_167</t>
+  </si>
+  <si>
+    <t>tc_toutpk_168</t>
+  </si>
+  <si>
+    <t>tc_toutpk_169</t>
+  </si>
+  <si>
+    <t>tc_toutpk_170</t>
+  </si>
+  <si>
+    <t>tc_toutpk_171</t>
+  </si>
+  <si>
+    <t>tc_toutpk_172</t>
+  </si>
+  <si>
+    <t>tc_toutpk_173</t>
+  </si>
+  <si>
+    <t>tc_toutpk_174</t>
+  </si>
+  <si>
+    <t>tc_toutpk_175</t>
+  </si>
+  <si>
+    <t>tc_toutpk_176</t>
+  </si>
+  <si>
+    <t>tc_toutpk_177</t>
+  </si>
+  <si>
+    <t>tc_toutpk_178</t>
+  </si>
+  <si>
+    <t>tc_toutpk_179</t>
+  </si>
+  <si>
+    <t>tc_toutpk_180</t>
+  </si>
+  <si>
+    <t>tc_toutpk_181</t>
+  </si>
+  <si>
+    <t>tc_toutpk_182</t>
+  </si>
+  <si>
+    <t>tc_toutpk_183</t>
+  </si>
+  <si>
+    <t>tc_toutpk_184</t>
+  </si>
+  <si>
+    <t>tc_toutpk_185</t>
+  </si>
+  <si>
+    <t>tc_toutpk_186</t>
+  </si>
+  <si>
+    <t>tc_toutpk_187</t>
+  </si>
+  <si>
+    <t>tc_toutpk_188</t>
+  </si>
+  <si>
+    <t>tc_toutpk_189</t>
+  </si>
+  <si>
+    <t>tc_toutpk_190</t>
+  </si>
+  <si>
+    <t>tc_toutpk_191</t>
+  </si>
+  <si>
+    <t>tc_toutpk_192</t>
+  </si>
+  <si>
+    <t>tc_toutpk_193</t>
+  </si>
+  <si>
+    <t>tc_toutpk_194</t>
+  </si>
+  <si>
+    <t>tc_toutpk_195</t>
+  </si>
+  <si>
+    <t>tc_toutpk_196</t>
+  </si>
+  <si>
+    <t>tc_toutpk_197</t>
+  </si>
+  <si>
+    <t>tc_toutpk_198</t>
+  </si>
+  <si>
+    <t>tc_toutpk_199</t>
+  </si>
+  <si>
+    <t>tc_toutpk_200</t>
+  </si>
+  <si>
+    <t>tc_toutpk_201</t>
+  </si>
+  <si>
+    <t>tc_toutpk_202</t>
+  </si>
+  <si>
+    <t>tc_toutpk_203</t>
+  </si>
+  <si>
+    <t>tc_toutpk_204</t>
+  </si>
+  <si>
+    <t>tc_toutpk_205</t>
+  </si>
+  <si>
+    <t>tc_toutpk_206</t>
+  </si>
+  <si>
+    <t>tc_toutpk_207</t>
+  </si>
+  <si>
+    <t>tc_toutpk_208</t>
+  </si>
+  <si>
+    <t>tc_toutpk_209</t>
+  </si>
+  <si>
+    <t>tc_toutpk_210</t>
+  </si>
+  <si>
+    <t>tc_toutpk_211</t>
+  </si>
+  <si>
+    <t>tc_toutpk_212</t>
+  </si>
+  <si>
+    <t>tc_toutpk_213</t>
+  </si>
+  <si>
+    <t>tc_toutpk_214</t>
+  </si>
+  <si>
+    <t>tc_toutpk_215</t>
+  </si>
+  <si>
+    <t>tc_toutpk_216</t>
+  </si>
+  <si>
+    <t>tc_toutpk_217</t>
+  </si>
+  <si>
+    <t>tc_toutpk_218</t>
+  </si>
+  <si>
+    <t>tc_toutpk_219</t>
+  </si>
+  <si>
+    <t>tc_toutpk_220</t>
+  </si>
+  <si>
+    <t>tc_toutpk_221</t>
+  </si>
+  <si>
+    <t>tc_toutpk_222</t>
+  </si>
+  <si>
+    <t>tc_toutpk_223</t>
+  </si>
+  <si>
+    <t>tc_toutpk_224</t>
+  </si>
+  <si>
+    <t>tc_toutpk_225</t>
+  </si>
+  <si>
+    <t>tc_toutpk_226</t>
+  </si>
+  <si>
+    <t>tc_toutpk_227</t>
+  </si>
+  <si>
+    <t>tc_toutpk_228</t>
+  </si>
+  <si>
+    <t>tc_toutpk_229</t>
+  </si>
+  <si>
+    <t>tc_toutpk_230</t>
+  </si>
+  <si>
+    <t>tc_toutpk_231</t>
+  </si>
+  <si>
+    <t>tc_toutpk_232</t>
+  </si>
+  <si>
+    <t>tc_toutpk_233</t>
+  </si>
+  <si>
+    <t>tc_toutpk_234</t>
+  </si>
+  <si>
+    <t>tc_toutpk_235</t>
+  </si>
+  <si>
+    <t>tc_toutpk_236</t>
+  </si>
+  <si>
+    <t>tc_toutpk_237</t>
+  </si>
+  <si>
+    <t>tc_toutpk_238</t>
+  </si>
+  <si>
+    <t>tc_toutpk_239</t>
+  </si>
+  <si>
+    <t>tc_toutpk_240</t>
+  </si>
+  <si>
+    <t>tc_toutpk_241</t>
+  </si>
+  <si>
+    <t>tc_toutpk_242</t>
+  </si>
+  <si>
+    <t>tc_toutpk_243</t>
+  </si>
+  <si>
+    <t>tc_toutpk_244</t>
+  </si>
+  <si>
+    <t>tc_toutpk_245</t>
+  </si>
+  <si>
+    <t>tc_toutpk_246</t>
+  </si>
+  <si>
+    <t>tc_toutpk_247</t>
+  </si>
+  <si>
+    <t>tc_toutpk_248</t>
+  </si>
+  <si>
+    <t>tc_toutpk_249</t>
+  </si>
+  <si>
+    <t>tc_toutpk_250</t>
+  </si>
+  <si>
+    <t>tc_toutpk_251</t>
+  </si>
+  <si>
+    <t>valid email invalid password</t>
+  </si>
+  <si>
+    <t>the system should stop from
+log in to the app and show a proper
+ error message that invalid passoword</t>
+  </si>
+  <si>
+    <t>invalid emal valid password</t>
+  </si>
+  <si>
+    <t>invalid email invalid password</t>
+  </si>
+  <si>
+    <t>1. go to the login page
+2. enter email
+3. enter password
+4. click on the submit button</t>
+  </si>
+  <si>
+    <t>invalid emial no password</t>
+  </si>
+  <si>
+    <t>no email no password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">case sensitive </t>
+  </si>
+  <si>
+    <t>password is case-sensitive</t>
+  </si>
+  <si>
+    <t>emial is case-sensitive</t>
+  </si>
+  <si>
+    <t>min/max length</t>
+  </si>
+  <si>
+    <t>password with min/max length</t>
+  </si>
+  <si>
+    <t>Email  should  show 
+error message if a user directly tries
+ to enter the password</t>
+  </si>
+  <si>
+    <t>Client side ui
+mapping validation</t>
+  </si>
+  <si>
+    <t>Email and password fields should
+ throw an error message after
+ entering data with invalid format</t>
+  </si>
+  <si>
+    <t>keyvoard
+ mapping</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter email and passord and 
+then press Enter key does
+ it invoke submit </t>
+  </si>
+  <si>
+    <t>changed data</t>
+  </si>
+  <si>
+    <t>login with old password</t>
+  </si>
+  <si>
+    <t>tc_toutpk_252</t>
+  </si>
+  <si>
+    <t>tc_toutpk_253</t>
+  </si>
+  <si>
+    <t>tc_toutpk_254</t>
+  </si>
+  <si>
+    <t>tc_toutpk_255</t>
+  </si>
+  <si>
+    <t>tc_toutpk_256</t>
+  </si>
+  <si>
+    <t>check tap order</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,6 +985,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -164,7 +1023,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -174,6 +1033,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -509,10 +1371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7C1A861-C807-452C-AB17-3D0EA730F589}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G257"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,14 +1411,1408 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
       <c r="G2" t="s">
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>278</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>280</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>281</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>283</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>284</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>285</v>
+      </c>
+      <c r="C8" t="s">
+        <v>286</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
+        <v>287</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>288</v>
+      </c>
+      <c r="C10" t="s">
+        <v>289</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
+        <v>295</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>301</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G163" xr:uid="{08FA6C22-6166-4568-9B5B-B719B5088C4D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G164" xr:uid="{08FA6C22-6166-4568-9B5B-B719B5088C4D}">
       <formula1>"Pass,Fail"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
end to end testing done
</commit_message>
<xml_diff>
--- a/Test_Cases_TourToPK.xlsx
+++ b/Test_Cases_TourToPK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\University_Study\Final Year Project\FYP-2\Project\TourToPK-Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B22378-3A1E-4FC4-B645-424D0584E19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2D5E40-9873-43F0-96FC-84C9C5CD2168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7920" yWindow="0" windowWidth="12570" windowHeight="10920" xr2:uid="{EDDAB5D1-2AE6-43D3-8E96-778F7AC8E49F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{EDDAB5D1-2AE6-43D3-8E96-778F7AC8E49F}"/>
   </bookViews>
   <sheets>
     <sheet name="test_cases" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="309">
   <si>
     <t>Test_Case_ID</t>
   </si>
@@ -929,10 +929,6 @@
  entering data with invalid format</t>
   </si>
   <si>
-    <t>keyvoard
- mapping</t>
-  </si>
-  <si>
     <t xml:space="preserve">Enter email and passord and 
 then press Enter key does
  it invoke submit </t>
@@ -959,7 +955,31 @@
     <t>tc_toutpk_256</t>
   </si>
   <si>
-    <t>check tap order</t>
+    <t>sign up</t>
+  </si>
+  <si>
+    <t>sign up with already register emial</t>
+  </si>
+  <si>
+    <t>signup with tourtopk official email</t>
+  </si>
+  <si>
+    <t>signup with all required field 
+with correct value.</t>
+  </si>
+  <si>
+    <t>signup with all required field 
+with incorrect value.</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>keyword
+ mapping</t>
+  </si>
+  <si>
+    <t>check tab order</t>
   </si>
 </sst>
 </file>
@@ -1373,8 +1393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7C1A861-C807-452C-AB17-3D0EA730F589}">
   <dimension ref="A1:G257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1567,10 +1587,10 @@
         <v>38</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>293</v>
+        <v>307</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>282</v>
@@ -1582,7 +1602,7 @@
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>282</v>
@@ -1593,93 +1613,111 @@
         <v>40</v>
       </c>
       <c r="B15" t="s">
+        <v>294</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>295</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C17" s="5" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C18" s="5" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C19" s="5" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C20" s="5" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>57</v>
       </c>
@@ -2786,27 +2824,27 @@
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update in Test cases
</commit_message>
<xml_diff>
--- a/Test_Cases_TourToPK.xlsx
+++ b/Test_Cases_TourToPK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\University_Study\Final Year Project\FYP-2\Project\TourToPK-Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2D5E40-9873-43F0-96FC-84C9C5CD2168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C87237D-6319-4726-9ECD-2D0FA8A723D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{EDDAB5D1-2AE6-43D3-8E96-778F7AC8E49F}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="346">
   <si>
     <t>Test_Case_ID</t>
   </si>
@@ -169,12 +169,6 @@
     <t>tc_toutpk_16</t>
   </si>
   <si>
-    <t>tc_toutpk_17</t>
-  </si>
-  <si>
-    <t>tc_toutpk_18</t>
-  </si>
-  <si>
     <t>tc_toutpk_19</t>
   </si>
   <si>
@@ -184,13 +178,7 @@
     <t>tc_toutpk_21</t>
   </si>
   <si>
-    <t>tc_toutpk_22</t>
-  </si>
-  <si>
     <t>tc_toutpk_23</t>
-  </si>
-  <si>
-    <t>tc_toutpk_24</t>
   </si>
   <si>
     <t>tc_toutpk_25</t>
@@ -964,22 +952,315 @@
     <t>signup with tourtopk official email</t>
   </si>
   <si>
-    <t>signup with all required field 
-with correct value.</t>
-  </si>
-  <si>
-    <t>signup with all required field 
-with incorrect value.</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
     <t>keyword
  mapping</t>
   </si>
   <si>
     <t>check tab order</t>
+  </si>
+  <si>
+    <t>Verify email verification is sent 
+after sign-up.</t>
+  </si>
+  <si>
+    <t>Verify users can request a
+ password reset.</t>
+  </si>
+  <si>
+    <t>Verify email is sent with
+ password reset instructions</t>
+  </si>
+  <si>
+    <t>Verify tourists can view and 
+update their profile</t>
+  </si>
+  <si>
+    <t>Verify tourists can access the home 
+page and see popular places, hotels, and
+ recommended plans</t>
+  </si>
+  <si>
+    <t>Verify tourists can search for places
+ and filter results.</t>
+  </si>
+  <si>
+    <t>Verify tourists can view details of a 
+the specific place and leave ratings and
+ reviews</t>
+  </si>
+  <si>
+    <t>Verify tourists can like a place and 
+see it in their liked places.</t>
+  </si>
+  <si>
+    <t>Verify tourist can create a custom tour 
+plan and download it as a PDF.</t>
+  </si>
+  <si>
+    <t>Verify tourist receives email notifications
+ for bookings and updates</t>
+  </si>
+  <si>
+    <t>Verify static pages load correctly and 
+display the appropriate content</t>
+  </si>
+  <si>
+    <t>Verify admin functionalities for managing
+ places, recommended plans, hotels,
+ packages, and user accounts</t>
+  </si>
+  <si>
+    <t>Verify tourists can use the contact form 
+to reach hotel managers and tour operators
+, and queries are acknowledged.</t>
+  </si>
+  <si>
+    <t>Verify content manager functionalities
+ for managing places and recommended 
+plans.</t>
+  </si>
+  <si>
+    <t>Verify hotel manager functionalities 
+for managing hotels and viewing bookings.</t>
+  </si>
+  <si>
+    <t>1. go to the login page
+2. enter email
+3. enter old password
+4. click on the submit button</t>
+  </si>
+  <si>
+    <t>1. Go sign up page
+2. Enter Name: Ahmed Mujtaba
+3. Enter the Email: ahmedmujtaba.cs@gmail.com
+4. Enter Phone: 03174197940
+5. Enter CNIC: 35200-3255024-1
+6. Enter Password: Programmer@123
+7. Enter Confirm Password: Programmer@123
+8. click on submit button</t>
+  </si>
+  <si>
+    <t>1. Go sign up page
+2. Enter Name: Ahmed Mujtaba
+3. Enter the Email: tourtopk.official@gmail.com
+4. Enter Phone: 03174197940
+5. Enter CNIC: 35200-3255024-1
+6. Enter Password: Programmer@123
+7. Enter Confirm Password: Programmer@123
+8.Click on submit button</t>
+  </si>
+  <si>
+    <t>1. go to the email box and check email from tourtopk.official@gmail.com
+2. Enter the pin code received on the email
+3. click on the submit button</t>
+  </si>
+  <si>
+    <t>1. Go to the login page
+2. click on forget password button
+3. Enter your registered email
+4. verify your email from pin code
+5. Enter New password
+6. Enter comfirm password
+7. Click on submit button</t>
+  </si>
+  <si>
+    <t>Verify user receives an email verificationde pin co after sign-up.</t>
+  </si>
+  <si>
+    <t>Verify error message is shown for 
+expired or invalid verification code.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Go to the home page of TourToPK
+2. Click on the Profile button
+3. View and update their information 
+4. Click on the save change button
+</t>
+  </si>
+  <si>
+    <t>1. Go to the Places Listing page
+2. Search by place title or by entering a city name
+3. Apply filters by Province, Place Type, and Order by rating and liked 
+places.</t>
+  </si>
+  <si>
+    <t>1. Go to the Places Listing page
+2. Click on the Places card 
+3. Choose a Rating star
+4. Write a review in the comment section
+5. Click on the submit button</t>
+  </si>
+  <si>
+    <t>1. Go to the Places Listing page 
+2. Click the heart icon on the Place card
+3. Click on the “Are you sure” button on the popup</t>
+  </si>
+  <si>
+    <t>Verify tourists can search for hotels, filter 
+results, view hotel details, book hotels.</t>
+  </si>
+  <si>
+    <t>1. Go to the hotel Listing page
+2. Search by hotel name
+3. Apply filters by Province, Price Range, and Order by rating and 
+expensive, cheapest hotel.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify tourists can search for hotels, filterresults, view hotel details, book hotels. </t>
+  </si>
+  <si>
+    <t>1. Go to the Hotel Listing page
+2. Click on the Hotel card 
+3. Click on the Booking button
+4. Enter Full Name: Ahmed Mujtaba
+5. Enter Email: ahmedmujtaba942kips@gmail.com
+6. Enter Phone: 03174197940
+7. Enter Number of Guests: 1
+8. Enter Address: LDA Avenue
+9. Enter Check -in-data: 05/06/2024
+10. Enter Check-out-date: 08/06/2024
+11. Enter City: Lahore
+12. Enter County: Pakistan
+13. Enter Special Request: AC must be working fine.
+14. Click on the next button for the payment method
+15. Enter Cardholder Name: Ahmed Mujtaba
+16. Enter Card Number: **** **** **** ****
+17. Enter MM/YY/ CVC: 03/25/***
+18. Click on submit button</t>
+  </si>
+  <si>
+    <t>1. Click on the Custom Tour butt
+2. Fill out your Personal information section
+3. Enter Full name: Ahmed Mujtaba
+4. Choose City: Lahore
+5. Enter Contact Number: 03174197940
+6. Choose Occupation: Student
+7. Enter Email: ahmedmujtaba942kips@gmail.com
+8. Enter Confirm Email: ahmedmujtaba942kips@gmail.com
+9. Fill out the Tour informational section
+10. Choose your preference: Standard
+11. Enter Budge: 80,000/-
+12. Enter start date: 05/06/2024
+13. Enter end date: 08/06/2024
+14. Enter Visitors: 5
+15. Enter adults: 5
+16. Enter children: 0
+17. Enter infants: 0
+18. Fill out the destination section
+19. Choose the tour location
+20. Select multiple places 
+21. Click on the submit button
+22. Click on the download button</t>
+  </si>
+  <si>
+    <t>1. go to enter email
+2. view booking details</t>
+  </si>
+  <si>
+    <t>1. Go to the Contact Us page
+2. Enter Full Name: Ahmed Mujtaba
+3. Enter Email: ahmedmujtaba942kips@gmail.com
+4. Enter Subject: how to register my hotel
+5. Enter Message: Hello, I want to register my hotel….
+6. Click on the send email button</t>
+  </si>
+  <si>
+    <t>1. Go to the login Page
+2. Enter Username: Admin 
+3. Enter password: *********
+4. Click on Sign-in button
+5. Click on the Places button
+6. Click on the Plans button
+7. Click on the Hotels button
+8. Click on the Packages button</t>
+  </si>
+  <si>
+    <t>1. Go to the login Page
+2. Enter Username: Admin 
+3. Enter password: *********
+4. Click on Sign-in button
+5. Click on the Add Partners Button
+6. Enter Company Name: 
+7. Enter CNIC:
+8. Enter Email:
+9. Enter Phone:
+10. Choose Partner Type:
+11. Enter 4 digit random number 
+12. Choose Province:
+13. Choose City:
+14. Enter Location:
+15. Click on submit</t>
+  </si>
+  <si>
+    <t>super admin should able to create a partners accounts</t>
+  </si>
+  <si>
+    <t>The system should allow the super admin to create hotel manager or tour 
+operator accounts, CNIC should be unique and contain dashes, the same 
+email cannot be used for TO or HM, the user name should be unique, the 
+Phone number must contain 11 digits, Cities must correlate with the 
+respective province.</t>
+  </si>
+  <si>
+    <t>1. Go to the login Page
+2. Enter Email: manager@tourtopk.com
+3. Enter password: *********
+4. Click on Sign-in button
+5. Click on the Add Places button
+6. Enter place title: 
+7. Enter a description:
+8. Enter activities:
+9. Enter famous food:
+10. Choose Province:
+11. Choose City:
+12. Enter Location:
+13. Choose Place Type:
+14. Choose images:
+15. Click on submit
+To view, delete, and update click on the View Places button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The system should allow the content manager to add places, after submitting 
+places details page should navigate to the all places page where the content 
+manager can view, update, and delete places. </t>
+  </si>
+  <si>
+    <t>1. Go to the hotel manager's dashboard home
+2. Click on the add hotel button
+3. Enter hotel name: 
+4. Choose amenities:
+5. Enter a description:
+6. Enter the number of beds:
+7. Enter price per night:
+8. Enter the number of bathrooms:
+9. Enter the number of guests:
+10. Choose images:
+11. Click on submit
+To view, delete, and update click on the View Hotels button</t>
+  </si>
+  <si>
+    <t>The system should allow the verified hotel manager to add a hotel, after 
+submitting the hotel details page should navigate to the all hotel page where 
+the hotel manager can view, update, and delete hotels. The hotel name 
+should be alphabets, number of beds, number of bathrooms, number of 
+guests, price should be a valid positive number. Otherwise, systems should 
+show a proper error message.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify user able to give user preference </t>
+  </si>
+  <si>
+    <t>1. Go to the Places Listing page
+2. Click the Suggest Us button
+3. Enter the Place title
+4. Enter description
+5. Enter activities to do 
+6. Enter Famous food to eat
+7. Click on the submit button</t>
+  </si>
+  <si>
+    <t>The system should allow verified users to suggest the places. TourToPK 
+Content Manager can view and delete user preferences.</t>
   </si>
 </sst>
 </file>
@@ -1048,13 +1329,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1391,18 +1672,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7C1A861-C807-452C-AB17-3D0EA730F589}">
-  <dimension ref="A1:G257"/>
+  <dimension ref="A1:G253"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="32.140625" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" customWidth="1"/>
+    <col min="4" max="4" width="35" customWidth="1"/>
     <col min="5" max="5" width="21.85546875" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
@@ -1441,10 +1722,10 @@
       <c r="C2" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>25</v>
       </c>
       <c r="F2" t="s">
@@ -1459,13 +1740,13 @@
         <v>28</v>
       </c>
       <c r="C3" t="s">
+        <v>274</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>279</v>
+      <c r="E3" s="4" t="s">
+        <v>275</v>
       </c>
       <c r="F3" t="s">
         <v>26</v>
@@ -1479,10 +1760,16 @@
         <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>280</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>282</v>
+        <v>276</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1490,10 +1777,16 @@
         <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>281</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>282</v>
+        <v>277</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1501,10 +1794,16 @@
         <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>283</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>282</v>
+        <v>279</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1512,10 +1811,16 @@
         <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>284</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>282</v>
+        <v>280</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1523,13 +1828,19 @@
         <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C8" t="s">
-        <v>286</v>
-      </c>
-      <c r="D8" s="5" t="s">
         <v>282</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="F8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1537,10 +1848,13 @@
         <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>287</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>282</v>
+        <v>283</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="F9" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1548,256 +1862,464 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C10" t="s">
-        <v>289</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>282</v>
+        <v>285</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="F10" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>282</v>
+      <c r="B11" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="F11" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>292</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>282</v>
+      <c r="C12" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="F12" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>308</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>282</v>
+      <c r="B13" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="F13" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5" t="s">
-        <v>293</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="F14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>294</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="F15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="F16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="C17" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="F17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="C18" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="F18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="F19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="F20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="F21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="F22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="F23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="F24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="F25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C26" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="F26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="F28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="405" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="F29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="390" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="F30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C31" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="F31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C32" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="F32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C33" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="D33" s="4"/>
+    </row>
+    <row r="34" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C34" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="270" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C35" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="330" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C36" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C37" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="F37" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="240" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C38" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>73</v>
       </c>
@@ -2804,22 +3326,22 @@
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>274</v>
+        <v>292</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>275</v>
+        <v>293</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>276</v>
+        <v>294</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>277</v>
+        <v>295</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.25">
@@ -2827,30 +3349,10 @@
         <v>296</v>
       </c>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A254" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A255" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A256" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A257" t="s">
-        <v>300</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G164" xr:uid="{08FA6C22-6166-4568-9B5B-B719B5088C4D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G160" xr:uid="{08FA6C22-6166-4568-9B5B-B719B5088C4D}">
       <formula1>"Pass,Fail"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2874,20 +3376,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2904,7 +3406,7 @@
       <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C3" t="s">
@@ -2945,22 +3447,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>